<commit_message>
Added modification consent form
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_category.xlsx
+++ b/mosip_master/xlsx/doc_category.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Desktop\NIRA MASTERDATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{538DAF58-3BDD-4B53-9600-19AF9B8D975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1888BE-EF11-435D-950C-72A4543C5D39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3F7CCF4D-8218-47FF-82F6-EB07A560EBA0}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" xr2:uid="{3F7CCF4D-8218-47FF-82F6-EB07A560EBA0}"/>
   </bookViews>
   <sheets>
     <sheet name="doc_category" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="62">
   <si>
     <t>code</t>
   </si>
@@ -197,13 +197,22 @@
   </si>
   <si>
     <t>Proof Of Court Order</t>
+  </si>
+  <si>
+    <t>POMC</t>
+  </si>
+  <si>
+    <t>Proof Of Modification Consent</t>
+  </si>
+  <si>
+    <t>Proof of Modification Consent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,7 +689,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1058,13 +1069,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAEBCC2-B773-4107-AFE8-13DD4FA99942}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:K19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1131,7 +1144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1163,7 +1176,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1195,7 +1208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1227,7 +1240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1259,7 +1272,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1291,7 +1304,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1355,7 +1368,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1387,7 +1400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1419,7 +1432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1451,7 +1464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1483,7 +1496,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1515,7 +1528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1547,7 +1560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1579,7 +1592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1611,7 +1624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1640,6 +1653,38 @@
         <v>45634.749305555553</v>
       </c>
       <c r="J18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="3">
+        <v>45634.749305555553</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="3">
+        <v>45634.749305555553</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Schema folder contains: ui spec and ID schema (#11)
* added Schema

* updated all spec

* deleted folder

* pushed all chnages
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_category.xlsx
+++ b/mosip_master/xlsx/doc_category.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Desktop\NIRA MASTERDATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{538DAF58-3BDD-4B53-9600-19AF9B8D975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09B177A-5A26-4D32-A779-7049CF8A9BB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3F7CCF4D-8218-47FF-82F6-EB07A560EBA0}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" xr2:uid="{3F7CCF4D-8218-47FF-82F6-EB07A560EBA0}"/>
   </bookViews>
   <sheets>
     <sheet name="doc_category" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="80">
   <si>
     <t>code</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Proof of Birth</t>
   </si>
   <si>
-    <t>Proof date of birth of the person</t>
-  </si>
-  <si>
     <t>POC</t>
   </si>
   <si>
@@ -133,12 +130,6 @@
     <t>POS</t>
   </si>
   <si>
-    <t>Proof Of Signature</t>
-  </si>
-  <si>
-    <t>Proof of Signature</t>
-  </si>
-  <si>
     <t>POREG</t>
   </si>
   <si>
@@ -175,9 +166,6 @@
     <t>POLSD</t>
   </si>
   <si>
-    <t>Proof Of Legal Statutory Declaration</t>
-  </si>
-  <si>
     <t>POD</t>
   </si>
   <si>
@@ -197,13 +185,88 @@
   </si>
   <si>
     <t>Proof Of Court Order</t>
+  </si>
+  <si>
+    <t>OTH03</t>
+  </si>
+  <si>
+    <t>Other Document</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>POABD</t>
+  </si>
+  <si>
+    <t>Proof of Abandonment</t>
+  </si>
+  <si>
+    <t>Proof of birth</t>
+  </si>
+  <si>
+    <t>POIS</t>
+  </si>
+  <si>
+    <t>Proof of Introducer Signature</t>
+  </si>
+  <si>
+    <t>jagadeesh t</t>
+  </si>
+  <si>
+    <t>POLC</t>
+  </si>
+  <si>
+    <t>Proof of Legal Change</t>
+  </si>
+  <si>
+    <t>Legal Statement under Oath</t>
+  </si>
+  <si>
+    <t>POMC</t>
+  </si>
+  <si>
+    <t>Proof of Modification Consent</t>
+  </si>
+  <si>
+    <t>POOSD</t>
+  </si>
+  <si>
+    <t>Proof of other supporting document Issued by Government</t>
+  </si>
+  <si>
+    <t>Proof of other supporting document issued by govt</t>
+  </si>
+  <si>
+    <t>POPC</t>
+  </si>
+  <si>
+    <t>Proof of Police Confirmation</t>
+  </si>
+  <si>
+    <t>PORARS</t>
+  </si>
+  <si>
+    <t>Proof of residence and registration supportÂ </t>
+  </si>
+  <si>
+    <t>Residence and Registration supportÂ </t>
+  </si>
+  <si>
+    <t>Authorization Documents</t>
+  </si>
+  <si>
+    <t>POSD</t>
+  </si>
+  <si>
+    <t>Proof of other supporting document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,9 +743,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1058,13 +1122,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAEBCC2-B773-4107-AFE8-13DD4FA99942}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="7" max="7" width="18.25" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1131,47 +1203,47 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1">
-        <v>45634.749305555553</v>
+      <c r="G3" s="2">
+        <v>45565.669496388888</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1">
-        <v>45634.749305555553</v>
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1183,7 +1255,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
@@ -1195,15 +1267,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1214,28 +1286,28 @@
       <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1">
-        <v>45634.749305555553</v>
+      <c r="G5" s="2">
+        <v>45553.383614444443</v>
       </c>
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="1">
-        <v>45634.749305555553</v>
+      <c r="I5" s="2">
+        <v>45553.383702002313</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -1247,7 +1319,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
@@ -1259,48 +1331,48 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2">
+        <v>45575.334317650464</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1">
-        <v>45634.749305555553</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="1">
-        <v>45634.749305555553</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -1311,7 +1383,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H8" t="s">
         <v>16</v>
@@ -1323,15 +1395,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -1343,7 +1415,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H9" t="s">
         <v>16</v>
@@ -1355,15 +1427,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -1375,7 +1447,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H10" t="s">
         <v>16</v>
@@ -1387,15 +1459,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -1407,7 +1479,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H11" t="s">
         <v>16</v>
@@ -1419,15 +1491,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1439,7 +1511,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1451,15 +1523,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -1471,7 +1543,7 @@
         <v>16</v>
       </c>
       <c r="G13" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -1483,15 +1555,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -1500,30 +1572,30 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="1">
-        <v>45634.749305555553</v>
+        <v>63</v>
+      </c>
+      <c r="G14" s="2">
+        <v>45590.316647199077</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="1">
-        <v>45634.749305555553</v>
+        <v>63</v>
+      </c>
+      <c r="I14" s="2">
+        <v>45590.316859212966</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -1534,28 +1606,28 @@
       <c r="F15" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="1">
-        <v>45634.749305555553</v>
+      <c r="G15" s="2">
+        <v>45614.50859125</v>
       </c>
       <c r="H15" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="1">
-        <v>45634.749305555553</v>
+      <c r="I15" s="2">
+        <v>45614.508798113427</v>
       </c>
       <c r="J15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -1567,7 +1639,7 @@
         <v>16</v>
       </c>
       <c r="G16" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H16" t="s">
         <v>16</v>
@@ -1579,15 +1651,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -1599,7 +1671,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="1">
-        <v>45634.749305555553</v>
+        <v>45516.749305555553</v>
       </c>
       <c r="H17" t="s">
         <v>16</v>
@@ -1611,15 +1683,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -1631,15 +1703,335 @@
         <v>16</v>
       </c>
       <c r="G18" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="2">
+        <v>45557.385132488424</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="2">
+        <v>45546.402661550928</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="2">
+        <v>45546.40284412037</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="2">
+        <v>45560.544703749998</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="2">
+        <v>45611.393834247683</v>
+      </c>
+      <c r="J20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="2">
+        <v>45614.30081572917</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="2">
+        <v>45614.307864074071</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1">
         <v>45634.749305555553</v>
       </c>
-      <c r="H18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1">
         <v>45634.749305555553</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="2">
+        <v>45566.254968564812</v>
+      </c>
+      <c r="H24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="2">
+        <v>45566.258958530096</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="1">
+        <v>45634.749305555553</v>
+      </c>
+      <c r="J25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="1">
+        <v>45634.749305555553</v>
+      </c>
+      <c r="J26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1">
+        <v>45516.749305555553</v>
+      </c>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="2">
+        <v>45574.553623206019</v>
+      </c>
+      <c r="J27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="2">
+        <v>45611.391187141206</v>
+      </c>
+      <c r="H28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="2">
+        <v>45611.391489756941</v>
+      </c>
+      <c r="J28" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>